<commit_message>
rebuilt tags model (v2.1.0)
</commit_message>
<xml_diff>
--- a/dist/cosasmappings.xlsx
+++ b/dist/cosasmappings.xlsx
@@ -25,7 +25,7 @@
     <t>COSAS Mappings</t>
   </si>
   <si>
-    <t>Mapping tables for processing raw data into unified model terminology (v2.0.0, 2022-05-02)</t>
+    <t>Mapping tables for processing raw data into unified model terminology (v2.1.0, 2022-06-29)</t>
   </si>
   <si>
     <t>template</t>
@@ -115,61 +115,61 @@
     <t>Available in place of something else.</t>
   </si>
   <si>
+    <t>NCIT_C25516</t>
+  </si>
+  <si>
+    <t>NCIT_C65107</t>
+  </si>
+  <si>
+    <t>NCIT_C25415</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>extends</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>idAttribute</t>
+  </si>
+  <si>
+    <t>nillable</t>
+  </si>
+  <si>
+    <t>lookupAttribute</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>dataType</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25415</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25516</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C65107</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25415</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>package</t>
-  </si>
-  <si>
-    <t>abstract</t>
-  </si>
-  <si>
-    <t>extends</t>
-  </si>
-  <si>
-    <t>entity</t>
-  </si>
-  <si>
-    <t>idAttribute</t>
-  </si>
-  <si>
-    <t>nillable</t>
-  </si>
-  <si>
-    <t>lookupAttribute</t>
-  </si>
-  <si>
-    <t>tags</t>
-  </si>
-  <si>
-    <t>auto</t>
-  </si>
-  <si>
-    <t>dataType</t>
-  </si>
-  <si>
-    <t>NCIT:C25415</t>
-  </si>
-  <si>
-    <t>NCIT:C25516</t>
-  </si>
-  <si>
-    <t>NCIT:C65107</t>
   </si>
   <si>
     <t>NCIT</t>
@@ -781,7 +781,7 @@
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>32</v>
       </c>
       <c r="H2" t="b">
@@ -810,7 +810,7 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
       <c r="H3" t="b">
@@ -839,7 +839,7 @@
       <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>34</v>
       </c>
       <c r="H4" t="b">
@@ -965,11 +965,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1003,14 +998,14 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>51</v>
@@ -1023,14 +1018,14 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
       <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>51</v>
@@ -1043,14 +1038,14 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>51</v>
@@ -1064,15 +1059,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3" location="isAssociatedWith"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="C3" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6" location="isAssociatedWith"/>
-    <hyperlink ref="A4" r:id="rId7"/>
-    <hyperlink ref="C4" r:id="rId8"/>
-    <hyperlink ref="F4" r:id="rId9" location="isAssociatedWith"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2" location="isAssociatedWith"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4" location="isAssociatedWith"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="F4" r:id="rId6" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>